<commit_message>
[]Classification Agis - en cours [] Barre de Navigation en cours []Création d'un objet pour les operations du chap Palettisation
</commit_message>
<xml_diff>
--- a/apps/test/data_migration/ModeleExportClassification.xlsx
+++ b/apps/test/data_migration/ModeleExportClassification.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="955" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
+    <workbookView activeTab="0" firstSheet="0" showHorizontalScroll="true" showSheetTabs="true" showVerticalScroll="true" tabRatio="940" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" state="visible" r:id="rId2"/>
@@ -204,7 +204,7 @@
   <dimension ref="B4:I21"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="true" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="I7" activeCellId="0" pane="topLeft" sqref="I7"/>
+      <selection activeCell="E1" activeCellId="0" pane="topLeft" sqref="E:E"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.05"/>
@@ -213,7 +213,9 @@
     <col collapsed="false" hidden="false" max="2" min="2" style="0" width="14.9948979591837"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="0" width="15.1275510204082"/>
     <col collapsed="false" hidden="false" max="4" min="4" style="0" width="11.8979591836735"/>
-    <col collapsed="false" hidden="false" max="8" min="5" style="0" width="10.7295918367347"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="12.5714285714286"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="14.4540816326531"/>
+    <col collapsed="false" hidden="false" max="8" min="7" style="0" width="10.7295918367347"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="0" width="11.4183673469388"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="10.7295918367347"/>
   </cols>
@@ -278,7 +280,7 @@
         <v>0</v>
       </c>
     </row>
-    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.9" outlineLevel="0" r="7">
+    <row collapsed="false" customFormat="false" customHeight="false" hidden="false" ht="14.05" outlineLevel="0" r="7">
       <c r="B7" s="0" t="s">
         <v>9</v>
       </c>
@@ -594,7 +596,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="E:E A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -620,7 +622,7 @@
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView colorId="64" defaultGridColor="true" rightToLeft="false" showFormulas="false" showGridLines="true" showOutlineSymbols="true" showRowColHeaders="true" showZeros="true" tabSelected="false" topLeftCell="A1" view="normal" windowProtection="false" workbookViewId="0" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100">
-      <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
+      <selection activeCell="A1" activeCellId="1" pane="topLeft" sqref="E:E A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>